<commit_message>
added nre rationale for model output signatur, new rational for file management
</commit_message>
<xml_diff>
--- a/software/3D-CMCC-Forest-Model/tables/CO_mod_transpiration.xlsx
+++ b/software/3D-CMCC-Forest-Model/tables/CO_mod_transpiration.xlsx
@@ -143,7 +143,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="582" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="582" uniqueCount="86">
   <si>
     <t>YEAR</t>
   </si>
@@ -390,6 +390,18 @@
   <si>
     <t>FCO2st 8.5</t>
   </si>
+  <si>
+    <t>[CO2] 8.5</t>
+  </si>
+  <si>
+    <t>[CO2] 6.0</t>
+  </si>
+  <si>
+    <t>[CO2] 4.5</t>
+  </si>
+  <si>
+    <t>[CO2] 2.6</t>
+  </si>
 </sst>
 </file>
 
@@ -3120,31 +3132,31 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="251287040"/>
-        <c:axId val="252932096"/>
+        <c:axId val="104782464"/>
+        <c:axId val="105058688"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="251287040"/>
+        <c:axId val="104782464"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="252932096"/>
+        <c:crossAx val="105058688"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="252932096"/>
+        <c:axId val="105058688"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="l"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="251287040"/>
+        <c:crossAx val="104782464"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3157,7 +3169,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000044" l="0.7000000000000004" r="0.7000000000000004" t="0.75000000000000044" header="0.30000000000000021" footer="0.30000000000000021"/>
+    <c:pageMargins b="0.75000000000000056" l="0.70000000000000051" r="0.70000000000000051" t="0.75000000000000056" header="0.30000000000000027" footer="0.30000000000000027"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -3176,11 +3188,11 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'annual comparison'!$E$1</c:f>
+              <c:f>Foglio9!$B$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v> CET  no</c:v>
+                  <c:v>[CO2] 8.5</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -3188,323 +3200,646 @@
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>Foglio9!$A:$A</c:f>
+              <c:strCache>
+                <c:ptCount val="105"/>
+                <c:pt idx="0">
+                  <c:v>year</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1996</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1997</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1998</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1999</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2001</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2002</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2003</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2004</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2005</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2006</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2007</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2008</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2009</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>2010</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>2011</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>2012</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>2013</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>2014</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>2015</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>2016</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>2017</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>2018</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>2019</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>2020</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>2021</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>2022</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>2023</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>2024</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>2025</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>2026</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>2027</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>2028</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>2029</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>2030</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>2031</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>2032</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>2033</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>2034</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>2035</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>2036</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>2037</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>2038</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>2039</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>2040</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>2041</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>2042</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>2043</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>2044</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>2045</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>2046</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>2047</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>2048</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>2049</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>2050</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>2051</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>2052</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>2053</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>2054</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>2055</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>2056</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>2057</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>2058</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>2059</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>2060</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>2061</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>2062</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>2063</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>2064</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>2065</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>2066</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>2067</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>2068</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>2069</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>2070</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>2071</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>2072</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>2073</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>2074</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>2075</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>2076</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>2077</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>2078</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>2079</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>2080</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>2081</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>2082</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>2083</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>2084</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>2085</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>2086</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>2087</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>2088</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>2089</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>2090</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>2091</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>2092</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>2093</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>2094</c:v>
+                </c:pt>
+                <c:pt idx="100">
+                  <c:v>2095</c:v>
+                </c:pt>
+                <c:pt idx="101">
+                  <c:v>2096</c:v>
+                </c:pt>
+                <c:pt idx="102">
+                  <c:v>2097</c:v>
+                </c:pt>
+                <c:pt idx="103">
+                  <c:v>2098</c:v>
+                </c:pt>
+                <c:pt idx="104">
+                  <c:v>2099</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'annual comparison'!$E$2:$E$126</c:f>
+              <c:f>Foglio9!$B$2:$B$105</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="125"/>
+                <c:ptCount val="104"/>
                 <c:pt idx="0">
-                  <c:v>280.62290000000002</c:v>
+                  <c:v>361.46300000000002</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>350.78899999999999</c:v>
+                  <c:v>363.15499999999997</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>308.38150000000002</c:v>
+                  <c:v>365.32299999999998</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>293.0401</c:v>
+                  <c:v>367.34800000000001</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>306.38639999999998</c:v>
+                  <c:v>368.86500000000001</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>320.92110000000002</c:v>
+                  <c:v>370.46800000000002</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>340.95620000000002</c:v>
+                  <c:v>372.52300000000002</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>307.66399999999999</c:v>
+                  <c:v>374.76</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>288.74</c:v>
+                  <c:v>376.81299999999999</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>398.31529999999998</c:v>
+                  <c:v>378.81299999999999</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>434.03250000000003</c:v>
+                  <c:v>380.82799999999997</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>374.48910000000001</c:v>
+                  <c:v>382.77800000000002</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>334.70490000000001</c:v>
+                  <c:v>384.8</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>452.69850000000002</c:v>
+                  <c:v>387.012</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>412.18579999999997</c:v>
+                  <c:v>389.32400000000001</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>394.1431</c:v>
+                  <c:v>391.63799999999998</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>395.98910000000001</c:v>
+                  <c:v>394.00900000000001</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>381.77519999999998</c:v>
+                  <c:v>396.464</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>485.6857</c:v>
+                  <c:v>399.00400000000002</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>418.7441</c:v>
+                  <c:v>401.62799999999999</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>474.54309999999998</c:v>
+                  <c:v>404.32799999999997</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>441.25779999999997</c:v>
+                  <c:v>407.096</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>473.22460000000001</c:v>
+                  <c:v>409.92700000000002</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>499.07819999999998</c:v>
+                  <c:v>412.822</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>479.0136</c:v>
+                  <c:v>415.78</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>508.36540000000002</c:v>
+                  <c:v>418.79599999999999</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>440.00630000000001</c:v>
+                  <c:v>421.86399999999998</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>425.03609999999998</c:v>
+                  <c:v>424.995</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>508.11070000000001</c:v>
+                  <c:v>428.197</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>488.7518</c:v>
+                  <c:v>431.47500000000002</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>459.24119999999999</c:v>
+                  <c:v>434.82600000000002</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>521.18140000000005</c:v>
+                  <c:v>438.245</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>563.75319999999999</c:v>
+                  <c:v>441.721</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>494.60950000000003</c:v>
+                  <c:v>445.25099999999998</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>431.19940000000003</c:v>
+                  <c:v>448.83499999999998</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>497.83580000000001</c:v>
+                  <c:v>452.47399999999999</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>499.90129999999999</c:v>
+                  <c:v>456.17700000000002</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>516.35479999999995</c:v>
+                  <c:v>459.964</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>531.4905</c:v>
+                  <c:v>463.85199999999998</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>480.07369999999997</c:v>
+                  <c:v>467.85</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>498.59820000000002</c:v>
+                  <c:v>471.96</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>454.71179999999998</c:v>
+                  <c:v>476.18200000000002</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>550.55909999999994</c:v>
+                  <c:v>480.50799999999998</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>546.16729999999995</c:v>
+                  <c:v>484.92700000000002</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>532.94349999999997</c:v>
+                  <c:v>489.435</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>569.12620000000004</c:v>
+                  <c:v>494.03199999999998</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>536.0829</c:v>
+                  <c:v>498.73</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>551.21069999999997</c:v>
+                  <c:v>503.53</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>534.53920000000005</c:v>
+                  <c:v>508.43299999999999</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>490.18009999999998</c:v>
+                  <c:v>513.45600000000002</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>594.44600000000003</c:v>
+                  <c:v>518.61099999999999</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>558.72640000000001</c:v>
+                  <c:v>523.9</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>467.38060000000002</c:v>
+                  <c:v>529.32399999999996</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>534.74969999999996</c:v>
+                  <c:v>534.875</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>462.84859999999998</c:v>
+                  <c:v>540.54300000000001</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>570.08920000000001</c:v>
+                  <c:v>546.322</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>551.60979999999995</c:v>
+                  <c:v>552.21199999999999</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>540.19079999999997</c:v>
+                  <c:v>558.21199999999999</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>564.96849999999995</c:v>
+                  <c:v>564.31299999999999</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>523.72760000000005</c:v>
+                  <c:v>570.51700000000005</c:v>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>509.17520000000002</c:v>
+                  <c:v>576.84299999999996</c:v>
                 </c:pt>
                 <c:pt idx="61">
-                  <c:v>587.32939999999996</c:v>
+                  <c:v>583.30499999999995</c:v>
                 </c:pt>
                 <c:pt idx="62">
-                  <c:v>571.79629999999997</c:v>
+                  <c:v>589.90499999999997</c:v>
                 </c:pt>
                 <c:pt idx="63">
-                  <c:v>518.65989999999999</c:v>
+                  <c:v>596.64700000000005</c:v>
                 </c:pt>
                 <c:pt idx="64">
-                  <c:v>546.49940000000004</c:v>
+                  <c:v>603.52</c:v>
                 </c:pt>
                 <c:pt idx="65">
-                  <c:v>552.62670000000003</c:v>
+                  <c:v>610.51700000000005</c:v>
                 </c:pt>
                 <c:pt idx="66">
-                  <c:v>543.90340000000003</c:v>
+                  <c:v>617.60500000000002</c:v>
                 </c:pt>
                 <c:pt idx="67">
-                  <c:v>578.75400000000002</c:v>
+                  <c:v>624.76400000000001</c:v>
                 </c:pt>
                 <c:pt idx="68">
-                  <c:v>591.21029999999996</c:v>
+                  <c:v>631.995</c:v>
                 </c:pt>
                 <c:pt idx="69">
-                  <c:v>502.37729999999999</c:v>
+                  <c:v>639.29100000000005</c:v>
                 </c:pt>
                 <c:pt idx="70">
-                  <c:v>543.44179999999994</c:v>
+                  <c:v>646.65300000000002</c:v>
                 </c:pt>
                 <c:pt idx="71">
-                  <c:v>598.31439999999998</c:v>
+                  <c:v>654.09799999999996</c:v>
                 </c:pt>
                 <c:pt idx="72">
-                  <c:v>542.45600000000002</c:v>
+                  <c:v>661.64499999999998</c:v>
                 </c:pt>
                 <c:pt idx="73">
-                  <c:v>530.43499999999995</c:v>
+                  <c:v>669.30499999999995</c:v>
                 </c:pt>
                 <c:pt idx="74">
-                  <c:v>552.62279999999998</c:v>
+                  <c:v>677.07799999999997</c:v>
                 </c:pt>
                 <c:pt idx="75">
-                  <c:v>619.24770000000001</c:v>
+                  <c:v>684.95399999999995</c:v>
                 </c:pt>
                 <c:pt idx="76">
-                  <c:v>592.82569999999998</c:v>
+                  <c:v>692.90200000000004</c:v>
                 </c:pt>
                 <c:pt idx="77">
-                  <c:v>564.99919999999997</c:v>
+                  <c:v>700.89400000000001</c:v>
                 </c:pt>
                 <c:pt idx="78">
-                  <c:v>616.38480000000004</c:v>
+                  <c:v>708.93200000000002</c:v>
                 </c:pt>
                 <c:pt idx="79">
-                  <c:v>631.01959999999997</c:v>
+                  <c:v>717.01499999999999</c:v>
                 </c:pt>
                 <c:pt idx="80">
-                  <c:v>593.57939999999996</c:v>
+                  <c:v>725.13599999999997</c:v>
                 </c:pt>
                 <c:pt idx="81">
-                  <c:v>572.08000000000004</c:v>
+                  <c:v>733.30700000000002</c:v>
                 </c:pt>
                 <c:pt idx="82">
-                  <c:v>602.56460000000004</c:v>
+                  <c:v>741.524</c:v>
                 </c:pt>
                 <c:pt idx="83">
-                  <c:v>626.61620000000005</c:v>
+                  <c:v>749.80499999999995</c:v>
                 </c:pt>
                 <c:pt idx="84">
-                  <c:v>586.69500000000005</c:v>
+                  <c:v>758.18200000000002</c:v>
                 </c:pt>
                 <c:pt idx="85">
-                  <c:v>577.93269999999995</c:v>
+                  <c:v>766.64499999999998</c:v>
                 </c:pt>
                 <c:pt idx="86">
-                  <c:v>629.96159999999998</c:v>
+                  <c:v>775.17399999999998</c:v>
                 </c:pt>
                 <c:pt idx="87">
-                  <c:v>630.88630000000001</c:v>
+                  <c:v>783.75099999999998</c:v>
                 </c:pt>
                 <c:pt idx="88">
-                  <c:v>626.16499999999996</c:v>
+                  <c:v>792.36599999999999</c:v>
                 </c:pt>
                 <c:pt idx="89">
-                  <c:v>601.69219999999996</c:v>
+                  <c:v>801.01900000000001</c:v>
                 </c:pt>
                 <c:pt idx="90">
-                  <c:v>626.76099999999997</c:v>
+                  <c:v>809.71500000000003</c:v>
                 </c:pt>
                 <c:pt idx="91">
-                  <c:v>636.54489999999998</c:v>
+                  <c:v>818.42200000000003</c:v>
                 </c:pt>
                 <c:pt idx="92">
-                  <c:v>632.61670000000004</c:v>
+                  <c:v>827.15700000000004</c:v>
                 </c:pt>
                 <c:pt idx="93">
-                  <c:v>609.30240000000003</c:v>
+                  <c:v>835.95600000000002</c:v>
                 </c:pt>
                 <c:pt idx="94">
-                  <c:v>557.83479999999997</c:v>
+                  <c:v>844.80499999999995</c:v>
                 </c:pt>
                 <c:pt idx="95">
-                  <c:v>531.06859999999995</c:v>
+                  <c:v>853.72500000000002</c:v>
                 </c:pt>
                 <c:pt idx="96">
-                  <c:v>528.59119999999996</c:v>
+                  <c:v>862.726</c:v>
                 </c:pt>
                 <c:pt idx="97">
-                  <c:v>576.28189999999995</c:v>
+                  <c:v>871.77700000000004</c:v>
                 </c:pt>
                 <c:pt idx="98">
-                  <c:v>611.59690000000001</c:v>
+                  <c:v>880.86400000000003</c:v>
                 </c:pt>
                 <c:pt idx="99">
-                  <c:v>634.3818</c:v>
+                  <c:v>889.98199999999997</c:v>
                 </c:pt>
                 <c:pt idx="100">
-                  <c:v>645.10400000000004</c:v>
+                  <c:v>899.12400000000002</c:v>
                 </c:pt>
                 <c:pt idx="101">
-                  <c:v>594.92989999999998</c:v>
+                  <c:v>908.28899999999999</c:v>
                 </c:pt>
                 <c:pt idx="102">
-                  <c:v>595.99959999999999</c:v>
+                  <c:v>917.471</c:v>
                 </c:pt>
                 <c:pt idx="103">
-                  <c:v>672.79880000000003</c:v>
+                  <c:v>926.66499999999996</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3515,11 +3850,11 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'annual comparison'!$H$1</c:f>
+              <c:f>Foglio9!$D$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v> CET </c:v>
+                  <c:v>[CO2] 6.0</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -3527,355 +3862,2019 @@
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>Foglio9!$A:$A</c:f>
+              <c:strCache>
+                <c:ptCount val="105"/>
+                <c:pt idx="0">
+                  <c:v>year</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1996</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1997</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1998</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1999</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2001</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2002</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2003</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2004</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2005</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2006</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2007</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2008</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2009</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>2010</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>2011</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>2012</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>2013</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>2014</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>2015</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>2016</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>2017</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>2018</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>2019</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>2020</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>2021</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>2022</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>2023</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>2024</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>2025</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>2026</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>2027</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>2028</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>2029</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>2030</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>2031</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>2032</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>2033</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>2034</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>2035</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>2036</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>2037</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>2038</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>2039</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>2040</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>2041</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>2042</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>2043</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>2044</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>2045</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>2046</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>2047</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>2048</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>2049</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>2050</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>2051</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>2052</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>2053</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>2054</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>2055</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>2056</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>2057</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>2058</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>2059</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>2060</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>2061</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>2062</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>2063</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>2064</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>2065</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>2066</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>2067</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>2068</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>2069</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>2070</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>2071</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>2072</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>2073</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>2074</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>2075</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>2076</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>2077</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>2078</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>2079</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>2080</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>2081</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>2082</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>2083</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>2084</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>2085</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>2086</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>2087</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>2088</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>2089</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>2090</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>2091</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>2092</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>2093</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>2094</c:v>
+                </c:pt>
+                <c:pt idx="100">
+                  <c:v>2095</c:v>
+                </c:pt>
+                <c:pt idx="101">
+                  <c:v>2096</c:v>
+                </c:pt>
+                <c:pt idx="102">
+                  <c:v>2097</c:v>
+                </c:pt>
+                <c:pt idx="103">
+                  <c:v>2098</c:v>
+                </c:pt>
+                <c:pt idx="104">
+                  <c:v>2099</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'annual comparison'!$H$2:$H$126</c:f>
+              <c:f>Foglio9!$D$2:$D$105</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="125"/>
+                <c:ptCount val="104"/>
                 <c:pt idx="0">
-                  <c:v>291.70609999999999</c:v>
+                  <c:v>361.46300000000002</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>363.23270000000002</c:v>
+                  <c:v>363.15499999999997</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>317.03100000000001</c:v>
+                  <c:v>365.32299999999998</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>298.858</c:v>
+                  <c:v>367.34800000000001</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>311.86869999999999</c:v>
+                  <c:v>368.86500000000001</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>325.56009999999998</c:v>
+                  <c:v>370.46800000000002</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>344.7106</c:v>
+                  <c:v>372.52300000000002</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>310.18290000000002</c:v>
+                  <c:v>374.76</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>290.10739999999998</c:v>
+                  <c:v>376.81299999999999</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>399.17939999999999</c:v>
+                  <c:v>378.81299999999999</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>433.70690000000002</c:v>
+                  <c:v>380.82799999999997</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>373.11439999999999</c:v>
+                  <c:v>382.77800000000002</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>333.38119999999998</c:v>
+                  <c:v>384.8</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>449.9085</c:v>
+                  <c:v>387.012</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>407.14909999999998</c:v>
+                  <c:v>389.32400000000001</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>388.28769999999997</c:v>
+                  <c:v>391.63799999999998</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>389.45359999999999</c:v>
+                  <c:v>394.00900000000001</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>374.15370000000001</c:v>
+                  <c:v>396.464</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>473.85680000000002</c:v>
+                  <c:v>397.346</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>409.1431</c:v>
+                  <c:v>399.387</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>460.91849999999999</c:v>
+                  <c:v>401.41800000000001</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>438.16759999999999</c:v>
+                  <c:v>403.43099999999998</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>457.6037</c:v>
+                  <c:v>405.42500000000001</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>493.12079999999997</c:v>
+                  <c:v>407.40100000000001</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>477.9083</c:v>
+                  <c:v>409.36</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>501.22430000000003</c:v>
+                  <c:v>411.298</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>439.02080000000001</c:v>
+                  <c:v>413.21899999999999</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>417.65410000000003</c:v>
+                  <c:v>415.14400000000001</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>503.70870000000002</c:v>
+                  <c:v>417.08300000000003</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>475.9905</c:v>
+                  <c:v>419.036</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>456.8954</c:v>
+                  <c:v>421.00400000000002</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>517.38480000000004</c:v>
+                  <c:v>422.97800000000001</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>556.77629999999999</c:v>
+                  <c:v>424.95</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>494.16050000000001</c:v>
+                  <c:v>426.916</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>424.96030000000002</c:v>
+                  <c:v>428.87599999999998</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>500.55259999999998</c:v>
+                  <c:v>430.83199999999999</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>500.87909999999999</c:v>
+                  <c:v>432.80700000000002</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>487.15390000000002</c:v>
+                  <c:v>434.83100000000002</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>521.0924</c:v>
+                  <c:v>436.916</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>463.8032</c:v>
+                  <c:v>439.06799999999998</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>490.5179</c:v>
+                  <c:v>441.286</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>459.18579999999997</c:v>
+                  <c:v>443.56700000000001</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>512.37810000000002</c:v>
+                  <c:v>445.90300000000002</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>527.09609999999998</c:v>
+                  <c:v>448.28199999999998</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>524.71780000000001</c:v>
+                  <c:v>450.69799999999998</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>565.50840000000005</c:v>
+                  <c:v>453.15</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>523.00199999999995</c:v>
+                  <c:v>455.64499999999998</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>532.29110000000003</c:v>
+                  <c:v>458.18200000000002</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>518.19569999999999</c:v>
+                  <c:v>460.762</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>449.56880000000001</c:v>
+                  <c:v>463.40499999999997</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>562.48170000000005</c:v>
+                  <c:v>466.12</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>540.69119999999998</c:v>
+                  <c:v>468.90800000000002</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>448.7629</c:v>
+                  <c:v>471.76799999999997</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>508.19189999999998</c:v>
+                  <c:v>474.69200000000001</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>430.39940000000001</c:v>
+                  <c:v>477.67</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>547.23990000000003</c:v>
+                  <c:v>480.697</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>512.97249999999997</c:v>
+                  <c:v>483.77699999999999</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>500.4144</c:v>
+                  <c:v>486.916</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>548.05589999999995</c:v>
+                  <c:v>490.10300000000001</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>496.0532</c:v>
+                  <c:v>493.33800000000002</c:v>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>451.73509999999999</c:v>
+                  <c:v>496.642</c:v>
                 </c:pt>
                 <c:pt idx="61">
-                  <c:v>559.40700000000004</c:v>
+                  <c:v>500.02199999999999</c:v>
                 </c:pt>
                 <c:pt idx="62">
-                  <c:v>517.58000000000004</c:v>
+                  <c:v>503.483</c:v>
                 </c:pt>
                 <c:pt idx="63">
-                  <c:v>460.07209999999998</c:v>
+                  <c:v>507.02300000000002</c:v>
                 </c:pt>
                 <c:pt idx="64">
-                  <c:v>513.42629999999997</c:v>
+                  <c:v>510.63400000000001</c:v>
                 </c:pt>
                 <c:pt idx="65">
-                  <c:v>516.22619999999995</c:v>
+                  <c:v>514.30499999999995</c:v>
                 </c:pt>
                 <c:pt idx="66">
-                  <c:v>503.0729</c:v>
+                  <c:v>518.02700000000004</c:v>
                 </c:pt>
                 <c:pt idx="67">
-                  <c:v>527.94809999999995</c:v>
+                  <c:v>521.79700000000003</c:v>
                 </c:pt>
                 <c:pt idx="68">
-                  <c:v>561.38310000000001</c:v>
+                  <c:v>525.61900000000003</c:v>
                 </c:pt>
                 <c:pt idx="69">
-                  <c:v>451.48379999999997</c:v>
+                  <c:v>529.48599999999999</c:v>
                 </c:pt>
                 <c:pt idx="70">
-                  <c:v>496.5419</c:v>
+                  <c:v>533.4</c:v>
                 </c:pt>
                 <c:pt idx="71">
-                  <c:v>566.03009999999995</c:v>
+                  <c:v>537.38099999999997</c:v>
                 </c:pt>
                 <c:pt idx="72">
-                  <c:v>523.92219999999998</c:v>
+                  <c:v>541.44299999999998</c:v>
                 </c:pt>
                 <c:pt idx="73">
-                  <c:v>496.96559999999999</c:v>
+                  <c:v>545.58900000000006</c:v>
                 </c:pt>
                 <c:pt idx="74">
-                  <c:v>507.4658</c:v>
+                  <c:v>549.82000000000005</c:v>
                 </c:pt>
                 <c:pt idx="75">
-                  <c:v>565.61540000000002</c:v>
+                  <c:v>554.12900000000002</c:v>
                 </c:pt>
                 <c:pt idx="76">
-                  <c:v>541.41690000000006</c:v>
+                  <c:v>558.48599999999999</c:v>
                 </c:pt>
                 <c:pt idx="77">
-                  <c:v>523.20569999999998</c:v>
+                  <c:v>562.86699999999996</c:v>
                 </c:pt>
                 <c:pt idx="78">
-                  <c:v>552.07569999999998</c:v>
+                  <c:v>567.27200000000005</c:v>
                 </c:pt>
                 <c:pt idx="79">
-                  <c:v>590.44129999999996</c:v>
+                  <c:v>571.70100000000002</c:v>
                 </c:pt>
                 <c:pt idx="80">
-                  <c:v>534.01509999999996</c:v>
+                  <c:v>576.14599999999996</c:v>
                 </c:pt>
                 <c:pt idx="81">
-                  <c:v>514.97889999999995</c:v>
+                  <c:v>580.60599999999999</c:v>
                 </c:pt>
                 <c:pt idx="82">
-                  <c:v>542.53189999999995</c:v>
+                  <c:v>585.10500000000002</c:v>
                 </c:pt>
                 <c:pt idx="83">
-                  <c:v>563.1268</c:v>
+                  <c:v>589.65300000000002</c:v>
                 </c:pt>
                 <c:pt idx="84">
-                  <c:v>516.06230000000005</c:v>
+                  <c:v>594.25699999999995</c:v>
                 </c:pt>
                 <c:pt idx="85">
-                  <c:v>545.6875</c:v>
+                  <c:v>598.91800000000001</c:v>
                 </c:pt>
                 <c:pt idx="86">
-                  <c:v>560.48540000000003</c:v>
+                  <c:v>603.53800000000001</c:v>
                 </c:pt>
                 <c:pt idx="87">
-                  <c:v>537.83079999999995</c:v>
+                  <c:v>608.02</c:v>
                 </c:pt>
                 <c:pt idx="88">
-                  <c:v>541.25329999999997</c:v>
+                  <c:v>612.36400000000003</c:v>
                 </c:pt>
                 <c:pt idx="89">
-                  <c:v>522.93299999999999</c:v>
+                  <c:v>616.572</c:v>
                 </c:pt>
                 <c:pt idx="90">
-                  <c:v>573.09879999999998</c:v>
+                  <c:v>620.64800000000002</c:v>
                 </c:pt>
                 <c:pt idx="91">
-                  <c:v>551.48720000000003</c:v>
+                  <c:v>624.58299999999997</c:v>
                 </c:pt>
                 <c:pt idx="92">
-                  <c:v>532.87810000000002</c:v>
+                  <c:v>628.38099999999997</c:v>
                 </c:pt>
                 <c:pt idx="93">
-                  <c:v>530.83849999999995</c:v>
+                  <c:v>632.06500000000005</c:v>
                 </c:pt>
                 <c:pt idx="94">
-                  <c:v>466.91829999999999</c:v>
+                  <c:v>635.649</c:v>
                 </c:pt>
                 <c:pt idx="95">
-                  <c:v>422.9008</c:v>
+                  <c:v>639.14099999999996</c:v>
                 </c:pt>
                 <c:pt idx="96">
-                  <c:v>429.53890000000001</c:v>
+                  <c:v>642.59699999999998</c:v>
                 </c:pt>
                 <c:pt idx="97">
-                  <c:v>522.81230000000005</c:v>
+                  <c:v>646.06100000000004</c:v>
                 </c:pt>
                 <c:pt idx="98">
-                  <c:v>543.20839999999998</c:v>
+                  <c:v>649.51499999999999</c:v>
                 </c:pt>
                 <c:pt idx="99">
-                  <c:v>554.04930000000002</c:v>
+                  <c:v>652.95100000000002</c:v>
                 </c:pt>
                 <c:pt idx="100">
-                  <c:v>563.70579999999995</c:v>
+                  <c:v>656.36400000000003</c:v>
                 </c:pt>
                 <c:pt idx="101">
-                  <c:v>518.52779999999996</c:v>
+                  <c:v>659.75400000000002</c:v>
                 </c:pt>
                 <c:pt idx="102">
-                  <c:v>497.89460000000003</c:v>
+                  <c:v>663.10699999999997</c:v>
                 </c:pt>
                 <c:pt idx="103">
-                  <c:v>571.19380000000001</c:v>
+                  <c:v>666.423</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Foglio9!$F$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>[CO2] 4.5</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>Foglio9!$A:$A</c:f>
+              <c:strCache>
+                <c:ptCount val="105"/>
+                <c:pt idx="0">
+                  <c:v>year</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1996</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1997</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1998</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1999</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2001</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2002</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2003</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2004</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2005</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2006</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2007</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2008</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2009</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>2010</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>2011</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>2012</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>2013</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>2014</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>2015</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>2016</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>2017</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>2018</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>2019</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>2020</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>2021</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>2022</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>2023</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>2024</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>2025</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>2026</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>2027</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>2028</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>2029</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>2030</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>2031</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>2032</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>2033</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>2034</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>2035</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>2036</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>2037</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>2038</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>2039</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>2040</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>2041</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>2042</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>2043</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>2044</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>2045</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>2046</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>2047</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>2048</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>2049</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>2050</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>2051</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>2052</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>2053</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>2054</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>2055</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>2056</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>2057</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>2058</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>2059</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>2060</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>2061</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>2062</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>2063</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>2064</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>2065</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>2066</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>2067</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>2068</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>2069</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>2070</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>2071</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>2072</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>2073</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>2074</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>2075</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>2076</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>2077</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>2078</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>2079</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>2080</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>2081</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>2082</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>2083</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>2084</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>2085</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>2086</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>2087</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>2088</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>2089</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>2090</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>2091</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>2092</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>2093</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>2094</c:v>
+                </c:pt>
+                <c:pt idx="100">
+                  <c:v>2095</c:v>
+                </c:pt>
+                <c:pt idx="101">
+                  <c:v>2096</c:v>
+                </c:pt>
+                <c:pt idx="102">
+                  <c:v>2097</c:v>
+                </c:pt>
+                <c:pt idx="103">
+                  <c:v>2098</c:v>
+                </c:pt>
+                <c:pt idx="104">
+                  <c:v>2099</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Foglio9!$F$2:$F$105</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="104"/>
+                <c:pt idx="0">
+                  <c:v>361.46300000000002</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>363.15499999999997</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>365.32299999999998</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>367.34800000000001</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>368.86500000000001</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>370.46800000000002</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>372.52300000000002</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>374.76</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>376.81299999999999</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>378.81299999999999</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>380.82799999999997</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>382.77800000000002</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>384.8</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>387.012</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>389.32400000000001</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>391.63799999999998</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>394.00900000000001</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>396.464</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>397.76400000000001</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>399.96600000000001</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>402.18400000000003</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>404.411</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>406.64299999999997</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>408.88200000000001</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>411.12900000000002</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>413.37799999999999</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>415.63900000000001</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>417.93599999999998</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>420.274</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>422.65600000000001</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>425.08</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>427.53800000000001</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>430.02100000000002</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>432.52300000000002</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>435.04599999999999</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>437.589</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>440.13099999999997</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>442.66399999999999</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>445.20699999999999</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>447.77</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>450.35500000000002</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>452.96300000000002</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>455.58600000000001</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>458.21499999999997</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>460.84500000000003</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>463.47500000000002</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>466.09300000000002</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>468.678</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>471.23399999999998</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>473.78</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>476.32799999999997</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>478.88099999999997</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>481.43799999999999</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>483.99299999999999</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>486.53500000000003</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>489.06</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>491.536</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>493.93200000000002</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>496.24400000000003</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>498.47399999999999</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>500.64499999999998</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>502.76799999999997</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>504.84699999999998</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>506.88400000000001</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>508.87099999999998</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>510.79899999999998</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>512.64700000000005</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>514.40200000000004</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>516.06500000000005</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>517.62900000000002</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>519.096</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>520.48800000000006</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>521.81799999999998</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>523.08900000000006</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>524.30200000000002</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>525.45100000000002</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>526.50900000000001</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>527.45699999999999</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>528.29600000000005</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>529.02700000000004</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>529.64300000000003</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>530.14400000000001</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>530.553</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>530.88300000000004</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>531.13800000000003</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>531.31899999999996</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>531.49</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>531.702</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>531.94200000000001</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>532.20500000000004</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>532.48699999999997</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>532.77599999999995</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>533.07000000000005</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>533.38800000000003</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>533.74099999999999</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>534.13099999999997</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>534.55799999999999</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>535.01099999999997</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>535.48</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>535.95500000000004</c:v>
+                </c:pt>
+                <c:pt idx="100">
+                  <c:v>536.43499999999995</c:v>
+                </c:pt>
+                <c:pt idx="101">
+                  <c:v>536.91999999999996</c:v>
+                </c:pt>
+                <c:pt idx="102">
+                  <c:v>537.399</c:v>
+                </c:pt>
+                <c:pt idx="103">
+                  <c:v>537.87099999999998</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Foglio9!$H$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>[CO2] 2.6</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>Foglio9!$A:$A</c:f>
+              <c:strCache>
+                <c:ptCount val="105"/>
+                <c:pt idx="0">
+                  <c:v>year</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1996</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1997</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1998</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1999</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2001</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2002</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2003</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2004</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2005</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2006</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2007</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2008</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2009</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>2010</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>2011</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>2012</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>2013</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>2014</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>2015</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>2016</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>2017</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>2018</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>2019</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>2020</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>2021</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>2022</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>2023</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>2024</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>2025</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>2026</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>2027</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>2028</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>2029</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>2030</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>2031</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>2032</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>2033</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>2034</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>2035</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>2036</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>2037</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>2038</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>2039</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>2040</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>2041</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>2042</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>2043</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>2044</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>2045</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>2046</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>2047</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>2048</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>2049</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>2050</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>2051</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>2052</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>2053</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>2054</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>2055</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>2056</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>2057</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>2058</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>2059</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>2060</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>2061</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>2062</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>2063</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>2064</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>2065</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>2066</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>2067</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>2068</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>2069</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>2070</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>2071</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>2072</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>2073</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>2074</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>2075</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>2076</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>2077</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>2078</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>2079</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>2080</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>2081</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>2082</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>2083</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>2084</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>2085</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>2086</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>2087</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>2088</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>2089</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>2090</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>2091</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>2092</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>2093</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>2094</c:v>
+                </c:pt>
+                <c:pt idx="100">
+                  <c:v>2095</c:v>
+                </c:pt>
+                <c:pt idx="101">
+                  <c:v>2096</c:v>
+                </c:pt>
+                <c:pt idx="102">
+                  <c:v>2097</c:v>
+                </c:pt>
+                <c:pt idx="103">
+                  <c:v>2098</c:v>
+                </c:pt>
+                <c:pt idx="104">
+                  <c:v>2099</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Foglio9!$H$2:$H$105</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="104"/>
+                <c:pt idx="0">
+                  <c:v>361.46300000000002</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>363.15499999999997</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>365.32299999999998</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>367.34800000000001</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>368.86500000000001</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>370.46800000000002</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>372.52300000000002</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>374.76</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>376.81299999999999</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>378.81299999999999</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>380.82799999999997</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>382.77800000000002</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>384.8</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>387.012</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>389.32400000000001</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>391.63799999999998</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>394.00900000000001</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>396.464</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>398.39600000000002</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>400.68099999999998</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>402.96800000000002</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>405.25200000000001</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>407.529</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>409.8</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>412.06799999999998</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>414.32600000000002</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>416.517</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>418.60300000000001</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>420.601</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>422.51600000000002</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>424.34899999999999</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>426.09699999999998</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>427.75200000000001</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>429.31400000000002</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>430.78300000000002</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>432.16300000000001</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>433.43599999999998</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>434.59300000000002</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>435.65300000000002</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>436.62799999999999</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>437.52199999999999</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>438.334</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>439.06</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>439.69099999999997</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>440.22199999999998</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>440.65699999999998</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>441.02499999999998</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>441.34699999999998</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>441.62099999999998</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>441.86399999999998</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>442.08499999999998</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>442.28300000000002</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>442.45800000000003</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>442.601</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>442.7</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>442.75200000000001</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>442.76100000000002</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>442.73399999999998</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>442.66300000000001</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>442.548</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>442.40600000000001</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>442.24799999999999</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>442.07499999999999</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>441.88600000000002</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>441.673</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>441.42399999999998</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>441.13499999999999</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>440.803</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>440.43</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>440.01</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>439.54500000000002</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>439.05200000000002</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>438.54300000000001</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>438.01900000000001</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>437.48099999999999</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>436.91899999999998</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>436.34300000000002</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>435.76400000000001</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>435.18200000000002</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>434.59500000000003</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>433.995</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>433.38499999999999</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>432.78</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>432.19</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>431.61700000000002</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>431.05799999999999</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>430.51</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>429.964</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>429.41399999999999</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>428.85899999999998</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>428.29899999999998</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>427.72699999999998</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>427.14299999999997</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>426.56599999999997</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>426.005</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>425.46100000000001</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>424.93700000000001</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>424.43099999999998</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>423.93099999999998</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>423.43099999999998</c:v>
+                </c:pt>
+                <c:pt idx="100">
+                  <c:v>422.92899999999997</c:v>
+                </c:pt>
+                <c:pt idx="101">
+                  <c:v>422.428</c:v>
+                </c:pt>
+                <c:pt idx="102">
+                  <c:v>421.91800000000001</c:v>
+                </c:pt>
+                <c:pt idx="103">
+                  <c:v>421.40100000000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="61201024"/>
-        <c:axId val="61219200"/>
+        <c:axId val="109703168"/>
+        <c:axId val="109704704"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="61201024"/>
+        <c:axId val="109703168"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="61219200"/>
+        <c:crossAx val="109704704"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="61219200"/>
+        <c:axId val="109704704"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="l"/>
-        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>[CO2](ppmv)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="61201024"/>
+        <c:crossAx val="109703168"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3907,6 +5906,736 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
+              <c:f>'annual comparison'!$E$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v> CET  no</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>'annual comparison'!$E$2:$E$126</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="125"/>
+                <c:pt idx="0">
+                  <c:v>280.62290000000002</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>350.78899999999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>308.38150000000002</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>293.0401</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>306.38639999999998</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>320.92110000000002</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>340.95620000000002</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>307.66399999999999</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>288.74</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>398.31529999999998</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>434.03250000000003</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>374.48910000000001</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>334.70490000000001</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>452.69850000000002</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>412.18579999999997</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>394.1431</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>395.98910000000001</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>381.77519999999998</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>485.6857</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>418.7441</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>474.54309999999998</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>441.25779999999997</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>473.22460000000001</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>499.07819999999998</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>479.0136</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>508.36540000000002</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>440.00630000000001</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>425.03609999999998</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>508.11070000000001</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>488.7518</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>459.24119999999999</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>521.18140000000005</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>563.75319999999999</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>494.60950000000003</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>431.19940000000003</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>497.83580000000001</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>499.90129999999999</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>516.35479999999995</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>531.4905</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>480.07369999999997</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>498.59820000000002</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>454.71179999999998</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>550.55909999999994</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>546.16729999999995</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>532.94349999999997</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>569.12620000000004</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>536.0829</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>551.21069999999997</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>534.53920000000005</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>490.18009999999998</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>594.44600000000003</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>558.72640000000001</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>467.38060000000002</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>534.74969999999996</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>462.84859999999998</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>570.08920000000001</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>551.60979999999995</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>540.19079999999997</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>564.96849999999995</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>523.72760000000005</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>509.17520000000002</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>587.32939999999996</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>571.79629999999997</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>518.65989999999999</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>546.49940000000004</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>552.62670000000003</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>543.90340000000003</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>578.75400000000002</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>591.21029999999996</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>502.37729999999999</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>543.44179999999994</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>598.31439999999998</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>542.45600000000002</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>530.43499999999995</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>552.62279999999998</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>619.24770000000001</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>592.82569999999998</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>564.99919999999997</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>616.38480000000004</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>631.01959999999997</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>593.57939999999996</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>572.08000000000004</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>602.56460000000004</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>626.61620000000005</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>586.69500000000005</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>577.93269999999995</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>629.96159999999998</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>630.88630000000001</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>626.16499999999996</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>601.69219999999996</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>626.76099999999997</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>636.54489999999998</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>632.61670000000004</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>609.30240000000003</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>557.83479999999997</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>531.06859999999995</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>528.59119999999996</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>576.28189999999995</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>611.59690000000001</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>634.3818</c:v>
+                </c:pt>
+                <c:pt idx="100">
+                  <c:v>645.10400000000004</c:v>
+                </c:pt>
+                <c:pt idx="101">
+                  <c:v>594.92989999999998</c:v>
+                </c:pt>
+                <c:pt idx="102">
+                  <c:v>595.99959999999999</c:v>
+                </c:pt>
+                <c:pt idx="103">
+                  <c:v>672.79880000000003</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'annual comparison'!$H$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v> CET </c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>'annual comparison'!$H$2:$H$126</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="125"/>
+                <c:pt idx="0">
+                  <c:v>291.70609999999999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>363.23270000000002</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>317.03100000000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>298.858</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>311.86869999999999</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>325.56009999999998</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>344.7106</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>310.18290000000002</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>290.10739999999998</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>399.17939999999999</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>433.70690000000002</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>373.11439999999999</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>333.38119999999998</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>449.9085</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>407.14909999999998</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>388.28769999999997</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>389.45359999999999</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>374.15370000000001</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>473.85680000000002</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>409.1431</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>460.91849999999999</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>438.16759999999999</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>457.6037</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>493.12079999999997</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>477.9083</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>501.22430000000003</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>439.02080000000001</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>417.65410000000003</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>503.70870000000002</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>475.9905</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>456.8954</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>517.38480000000004</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>556.77629999999999</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>494.16050000000001</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>424.96030000000002</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>500.55259999999998</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>500.87909999999999</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>487.15390000000002</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>521.0924</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>463.8032</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>490.5179</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>459.18579999999997</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>512.37810000000002</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>527.09609999999998</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>524.71780000000001</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>565.50840000000005</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>523.00199999999995</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>532.29110000000003</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>518.19569999999999</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>449.56880000000001</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>562.48170000000005</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>540.69119999999998</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>448.7629</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>508.19189999999998</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>430.39940000000001</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>547.23990000000003</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>512.97249999999997</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>500.4144</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>548.05589999999995</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>496.0532</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>451.73509999999999</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>559.40700000000004</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>517.58000000000004</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>460.07209999999998</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>513.42629999999997</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>516.22619999999995</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>503.0729</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>527.94809999999995</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>561.38310000000001</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>451.48379999999997</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>496.5419</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>566.03009999999995</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>523.92219999999998</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>496.96559999999999</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>507.4658</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>565.61540000000002</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>541.41690000000006</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>523.20569999999998</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>552.07569999999998</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>590.44129999999996</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>534.01509999999996</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>514.97889999999995</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>542.53189999999995</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>563.1268</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>516.06230000000005</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>545.6875</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>560.48540000000003</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>537.83079999999995</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>541.25329999999997</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>522.93299999999999</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>573.09879999999998</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>551.48720000000003</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>532.87810000000002</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>530.83849999999995</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>466.91829999999999</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>422.9008</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>429.53890000000001</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>522.81230000000005</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>543.20839999999998</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>554.04930000000002</c:v>
+                </c:pt>
+                <c:pt idx="100">
+                  <c:v>563.70579999999995</c:v>
+                </c:pt>
+                <c:pt idx="101">
+                  <c:v>518.52779999999996</c:v>
+                </c:pt>
+                <c:pt idx="102">
+                  <c:v>497.89460000000003</c:v>
+                </c:pt>
+                <c:pt idx="103">
+                  <c:v>571.19380000000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:marker val="1"/>
+        <c:axId val="107787008"/>
+        <c:axId val="107788544"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="107787008"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="107788544"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="107788544"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="107787008"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="it-IT"/>
+  <c:chart>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
               <c:f>'annual comparison'!$B$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
@@ -4581,24 +7310,24 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="169596032"/>
-        <c:axId val="169597952"/>
+        <c:axId val="106371328"/>
+        <c:axId val="106393600"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="169596032"/>
+        <c:axId val="106371328"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="169597952"/>
+        <c:crossAx val="106393600"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="169597952"/>
+        <c:axId val="106393600"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4606,20 +7335,19 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="169596032"/>
+        <c:crossAx val="106371328"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -4655,6 +7383,74 @@
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>447675</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>142875</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Grafico 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>327660</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>99060</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Immagine 4"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3" cstate="print"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11096625" y="952500"/>
+          <a:ext cx="4594860" cy="2766060"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -10647,13 +13443,14 @@
   <dimension ref="A1:I105"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P10" sqref="P10"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.42578125" customWidth="1"/>
     <col min="4" max="4" width="9.5703125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9.5703125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="9.5703125" bestFit="1" customWidth="1"/>
@@ -10664,25 +13461,25 @@
         <v>62</v>
       </c>
       <c r="B1" t="s">
-        <v>63</v>
+        <v>82</v>
       </c>
       <c r="C1" t="s">
         <v>81</v>
       </c>
       <c r="D1" t="s">
-        <v>72</v>
+        <v>83</v>
       </c>
       <c r="E1" t="s">
         <v>78</v>
       </c>
       <c r="F1" t="s">
-        <v>73</v>
+        <v>84</v>
       </c>
       <c r="G1" t="s">
         <v>79</v>
       </c>
       <c r="H1" t="s">
-        <v>76</v>
+        <v>85</v>
       </c>
       <c r="I1" t="s">
         <v>80</v>

</xml_diff>